<commit_message>
Updated link budget model to new format.
</commit_message>
<xml_diff>
--- a/modcods/modcods_dvbs2.xlsx
+++ b/modcods/modcods_dvbs2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\hermes-optimization\modcods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840B3124-77C6-4A40-BF26-3256AF19908C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2703CB3-8A54-48F7-9268-39B67E2BB480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{475A5499-7154-4666-96AD-43C3FB4797D8}"/>
   </bookViews>
@@ -658,7 +658,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q32" sqref="Q32"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B2," ",D2)</f>
+        <f t="shared" ref="E2:E29" si="0">_xlfn.CONCAT("DVB-S2 ",B2," ",D2)</f>
         <v xml:space="preserve">DVB-S2 QPSK 1/4 </v>
       </c>
       <c r="F2" s="7" t="str">
@@ -853,7 +853,7 @@
         <v>-2.35</v>
       </c>
       <c r="H2" s="4">
-        <f t="shared" ref="H2:H29" si="0">G2-10*LOG10(I2)</f>
+        <f t="shared" ref="H2:H29" si="1">G2-10*LOG10(I2)</f>
         <v>0.74588598747536183</v>
       </c>
       <c r="I2" s="5">
@@ -910,18 +910,18 @@
         <v>2</v>
       </c>
       <c r="E3" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B3," ",D3)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 QPSK 1/3 </v>
       </c>
       <c r="F3" s="7" t="str">
-        <f t="shared" ref="F3:F29" si="1">_xlfn.CONCAT("DVB_S2_",B3,"_",LEFT(D3, SEARCH("/", D3,1) - 1), "r", RIGHT(D3, LEN(D3) - SEARCH("/", D3,1) ))</f>
+        <f t="shared" ref="F3:F29" si="2">_xlfn.CONCAT("DVB_S2_",B3,"_",LEFT(D3, SEARCH("/", D3,1) - 1), "r", RIGHT(D3, LEN(D3) - SEARCH("/", D3,1) ))</f>
         <v xml:space="preserve">DVB_S2_QPSK_1r3 </v>
       </c>
       <c r="G3" s="2">
         <v>-1.24</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5879967049985575</v>
       </c>
       <c r="I3" s="5">
@@ -978,18 +978,18 @@
         <v>3</v>
       </c>
       <c r="E4" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B4," ",D4)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 QPSK 2/5 </v>
       </c>
       <c r="F4" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_QPSK_2r5 </v>
       </c>
       <c r="G4" s="2">
         <v>-0.3</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.72696276098380475</v>
       </c>
       <c r="I4" s="5">
@@ -1046,18 +1046,18 @@
         <v>4</v>
       </c>
       <c r="E5" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B5," ",D5)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 QPSK 1/2 </v>
       </c>
       <c r="F5" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">DVB_S2_QPSK_1r2 </v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">DVB_S2_QPSK_1r2 </v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4">
-        <f t="shared" si="0"/>
         <v>1.0486606860920165</v>
       </c>
       <c r="I5" s="5">
@@ -1114,18 +1114,18 @@
         <v>5</v>
       </c>
       <c r="E6" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B6," ",D6)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 QPSK 3/5 </v>
       </c>
       <c r="F6" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_QPSK_3r5 </v>
       </c>
       <c r="G6" s="2">
         <v>2.23</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4807244097668941</v>
       </c>
       <c r="I6" s="6">
@@ -1182,18 +1182,18 @@
         <v>6</v>
       </c>
       <c r="E7" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B7," ",D7)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 QPSK 2/3 </v>
       </c>
       <c r="F7" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_QPSK_2r3 </v>
       </c>
       <c r="G7" s="2">
         <v>3.1</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8868543895676191</v>
       </c>
       <c r="I7" s="6">
@@ -1250,18 +1250,18 @@
         <v>7</v>
       </c>
       <c r="E8" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B8," ",D8)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 QPSK 3/4 </v>
       </c>
       <c r="F8" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_QPSK_3r4 </v>
       </c>
       <c r="G8" s="2">
         <v>4.03</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.305509086632334</v>
       </c>
       <c r="I8" s="6">
@@ -1318,18 +1318,18 @@
         <v>8</v>
       </c>
       <c r="E9" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B9," ",D9)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 QPSK 4/5 </v>
       </c>
       <c r="F9" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_QPSK_4r5 </v>
       </c>
       <c r="G9" s="2">
         <v>4.68</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.6736943968341755</v>
       </c>
       <c r="I9" s="6">
@@ -1386,18 +1386,18 @@
         <v>9</v>
       </c>
       <c r="E10" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B10," ",D10)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 QPSK 5/6 </v>
       </c>
       <c r="F10" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_QPSK_5r6 </v>
       </c>
       <c r="G10" s="2">
         <v>5.18</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.9929044427101088</v>
       </c>
       <c r="I10" s="6">
@@ -1454,18 +1454,18 @@
         <v>10</v>
       </c>
       <c r="E11" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B11," ",D11)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 QPSK 8/9 </v>
       </c>
       <c r="F11" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_QPSK_8r9 </v>
       </c>
       <c r="G11" s="2">
         <v>6.2</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7289840505889056</v>
       </c>
       <c r="I11" s="6">
@@ -1522,18 +1522,18 @@
         <v>11</v>
       </c>
       <c r="E12" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B12," ",D12)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 QPSK 9/10 </v>
       </c>
       <c r="F12" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_QPSK_9r10 </v>
       </c>
       <c r="G12" s="2">
         <v>6.42</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8948385984320204</v>
       </c>
       <c r="I12" s="6">
@@ -1590,18 +1590,18 @@
         <v>5</v>
       </c>
       <c r="E13" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B13," ",D13)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 8PSK 3/5 </v>
       </c>
       <c r="F13" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_8PSK_3r5 </v>
       </c>
       <c r="G13" s="2">
         <v>5.5</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.9958219356763327</v>
       </c>
       <c r="I13" s="6">
@@ -1670,18 +1670,18 @@
         <v>6</v>
       </c>
       <c r="E14" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B14," ",D14)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 8PSK 2/3 </v>
       </c>
       <c r="F14" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_8PSK_2r3 </v>
       </c>
       <c r="G14" s="2">
         <v>6.62</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.6519533148655956</v>
       </c>
       <c r="I14" s="6">
@@ -1750,18 +1750,18 @@
         <v>7</v>
       </c>
       <c r="E15" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B15," ",D15)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 8PSK 3/4 </v>
       </c>
       <c r="F15" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_8PSK_3r4 </v>
       </c>
       <c r="G15" s="2">
         <v>7.91</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.4306064338285864</v>
       </c>
       <c r="I15" s="6">
@@ -1830,18 +1830,18 @@
         <v>9</v>
       </c>
       <c r="E16" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B16," ",D16)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 8PSK 5/6 </v>
       </c>
       <c r="F16" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_8PSK_5r6 </v>
       </c>
       <c r="G16" s="2">
         <v>9.35</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.4080021296173451</v>
       </c>
       <c r="I16" s="6">
@@ -1910,18 +1910,18 @@
         <v>10</v>
       </c>
       <c r="E17" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B17," ",D17)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 8PSK 8/9 </v>
       </c>
       <c r="F17" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_8PSK_8r9 </v>
       </c>
       <c r="G17" s="2">
         <v>10.69</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.464081905634969</v>
       </c>
       <c r="I17" s="6">
@@ -1990,18 +1990,18 @@
         <v>11</v>
       </c>
       <c r="E18" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B18," ",D18)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 8PSK 9/10 </v>
       </c>
       <c r="F18" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_8PSK_9r10 </v>
       </c>
       <c r="G18" s="2">
         <v>10.98</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6999373077969979</v>
       </c>
       <c r="I18" s="6">
@@ -2070,18 +2070,18 @@
         <v>6</v>
       </c>
       <c r="E19" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B19," ",D19)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 16APSK 2/3 </v>
       </c>
       <c r="F19" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_16APSK_2r3 </v>
       </c>
       <c r="G19" s="2">
         <v>8.9700000000000006</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.758567682482199</v>
       </c>
       <c r="I19" s="6">
@@ -2174,18 +2174,18 @@
         <v>7</v>
       </c>
       <c r="E20" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B20," ",D20)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 16APSK 3/4 </v>
       </c>
       <c r="F20" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_16APSK_3r4 </v>
       </c>
       <c r="G20" s="2">
         <v>10.210000000000001</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.487222694951269</v>
       </c>
       <c r="I20" s="6">
@@ -2278,18 +2278,18 @@
         <v>8</v>
       </c>
       <c r="E21" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B21," ",D21)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 16APSK 4/5 </v>
       </c>
       <c r="F21" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_16APSK_4r5 </v>
       </c>
       <c r="G21" s="2">
         <v>11.03</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.0254080734122093</v>
       </c>
       <c r="I21" s="6">
@@ -2382,18 +2382,18 @@
         <v>9</v>
       </c>
       <c r="E22" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B22," ",D22)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 16APSK 5/6 </v>
       </c>
       <c r="F22" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_16APSK_5r6 </v>
       </c>
       <c r="G22" s="2">
         <v>11.61</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.4246184558970221</v>
       </c>
       <c r="I22" s="6">
@@ -2486,18 +2486,18 @@
         <v>10</v>
       </c>
       <c r="E23" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B23," ",D23)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 16APSK 8/9 </v>
       </c>
       <c r="F23" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_16APSK_8r9 </v>
       </c>
       <c r="G23" s="2">
         <v>12.89</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4206972898721313</v>
       </c>
       <c r="I23" s="6">
@@ -2590,18 +2590,18 @@
         <v>11</v>
       </c>
       <c r="E24" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B24," ",D24)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 16APSK 9/10 </v>
       </c>
       <c r="F24" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_16APSK_9r10 </v>
       </c>
       <c r="G24" s="2">
         <v>13.13</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.6065525298491998</v>
       </c>
       <c r="I24" s="6">
@@ -2694,18 +2694,18 @@
         <v>7</v>
       </c>
       <c r="E25" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B25," ",D25)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 32APSK 3/4 </v>
       </c>
       <c r="F25" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_32APSK_3r4 </v>
       </c>
       <c r="G25" s="2">
         <v>12.73</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.0441169119948848</v>
       </c>
       <c r="I25" s="6">
@@ -2846,18 +2846,18 @@
         <v>8</v>
       </c>
       <c r="E26" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B26," ",D26)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 32APSK 4/5 </v>
       </c>
       <c r="F26" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_32APSK_4r5 </v>
       </c>
       <c r="G26" s="2">
         <v>13.64</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.6723021045227782</v>
       </c>
       <c r="I26" s="6">
@@ -2998,18 +2998,18 @@
         <v>9</v>
       </c>
       <c r="E27" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B27," ",D27)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 32APSK 5/6 </v>
       </c>
       <c r="F27" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_32APSK_5r6 </v>
       </c>
       <c r="G27" s="2">
         <v>14.28</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.1315127586371467</v>
       </c>
       <c r="I27" s="6">
@@ -3150,18 +3150,18 @@
         <v>10</v>
       </c>
       <c r="E28" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B28," ",D28)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 32APSK 8/9 </v>
       </c>
       <c r="F28" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_32APSK_8r9 </v>
       </c>
       <c r="G28" s="2">
         <v>15.69</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.2575919244836147</v>
       </c>
       <c r="I28" s="6">
@@ -3302,18 +3302,18 @@
         <v>11</v>
       </c>
       <c r="E29" s="7" t="str">
-        <f>_xlfn.CONCAT("DVB-S2 ",B29," ",D29)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">DVB-S2 32APSK 9/10 </v>
       </c>
       <c r="F29" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">DVB_S2_32APSK_9r10 </v>
       </c>
       <c r="G29" s="2">
         <v>16.05</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.5634467160682739</v>
       </c>
       <c r="I29" s="6">

</xml_diff>

<commit_message>
Did computations of sub-carrier aggregation.
</commit_message>
<xml_diff>
--- a/modcods/modcods_dvbs2.xlsx
+++ b/modcods/modcods_dvbs2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\hermes-optimization\modcods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2703CB3-8A54-48F7-9268-39B67E2BB480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC44726-F2E7-486E-ADA9-828AAE9B38AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{475A5499-7154-4666-96AD-43C3FB4797D8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{475A5499-7154-4666-96AD-43C3FB4797D8}"/>
   </bookViews>
   <sheets>
     <sheet name="DVB-S2" sheetId="1" r:id="rId1"/>
@@ -658,7 +658,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>